<commit_message>
Enhance invoice management with packagesCount field and regional handling
- Added packagesCount field to the InvoiceItem model for improved item tracking.
- Updated invoice routes to handle packagesCount in data transformations and validations.
- Implemented regional identification based on branch names in CMR and TIR Excel generation, enhancing document accuracy.
- Adjusted frontend Invoice component to include packagesCount in item management and validation logic, ensuring comprehensive data handling.
</commit_message>
<xml_diff>
--- a/backend/templates/TIR_template.xlsx
+++ b/backend/templates/TIR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Prodeklarant\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22EAB9B-0F13-4A40-9271-22365333920B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD6577B-A28E-47C4-87AB-D9E92FA4A6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Всего:</t>
   </si>
   <si>
-    <t xml:space="preserve">ИНВ № </t>
-  </si>
-  <si>
     <t>УЗБЕКИСТАН</t>
   </si>
   <si>
@@ -70,14 +67,17 @@
     <t>Ташкентская область</t>
   </si>
   <si>
-    <t xml:space="preserve">CMР №  </t>
+    <t>ИНВ №</t>
+  </si>
+  <si>
+    <t>CMР №</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,6 +214,19 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,21 +291,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -325,7 +332,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="11" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -336,7 +342,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="4"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -352,21 +382,6 @@
     </xf>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -814,11 +829,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Лист9"/>
+  <sheetPr codeName="Лист9">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:H19"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -826,27 +843,27 @@
     <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -859,17 +876,17 @@
       <c r="U1" s="2"/>
     </row>
     <row r="2" spans="1:21" ht="25.5" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -882,19 +899,19 @@
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="8"/>
-      <c r="B3" s="32" t="s">
-        <v>6</v>
+      <c r="A3" s="6"/>
+      <c r="B3" s="30" t="s">
+        <v>5</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -907,17 +924,17 @@
       <c r="U3" s="2"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="8"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -930,17 +947,17 @@
       <c r="U4" s="2"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="8"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -953,17 +970,17 @@
       <c r="U5" s="2"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -976,21 +993,20 @@
       <c r="U6" s="2"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>2</v>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>1</v>
       </c>
-      <c r="E7" s="33" t="s">
-        <v>5</v>
+      <c r="F7" s="27" t="s">
+        <v>4</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1003,17 +1019,17 @@
       <c r="U7" s="2"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1026,17 +1042,17 @@
       <c r="U8" s="2"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1049,20 +1065,20 @@
       <c r="U9" s="2"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19" t="s">
-        <v>1</v>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="23" t="s">
+        <v>6</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="23"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="20"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1074,20 +1090,20 @@
       <c r="U10" s="2"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="19" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="24"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="21"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1099,17 +1115,17 @@
       <c r="U11" s="2"/>
     </row>
     <row r="12" spans="1:21" ht="6" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1122,19 +1138,19 @@
       <c r="U12" s="2"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="8"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
-        <v>4</v>
+      <c r="A13" s="6"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>3</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1147,19 +1163,19 @@
       <c r="U13" s="2"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="19" t="s">
-        <v>4</v>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="17" t="s">
+        <v>3</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1172,17 +1188,17 @@
       <c r="U14" s="2"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1195,17 +1211,17 @@
       <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:21" ht="28.5" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="8"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1218,14 +1234,15 @@
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="3"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1238,14 +1255,15 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="3"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1258,14 +1276,15 @@
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="3"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1278,14 +1297,15 @@
       <c r="U19" s="2"/>
     </row>
     <row r="20" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="3"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1297,122 +1317,122 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="2:21" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-    </row>
-    <row r="22" spans="2:21" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-    </row>
-    <row r="23" spans="2:21" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="8"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-    </row>
-    <row r="24" spans="2:21" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="8"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-    </row>
-    <row r="25" spans="2:21" s="4" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="8"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
+    <row r="21" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="26"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="26"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+    </row>
+    <row r="24" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="26"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="26"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
     </row>
     <row r="26" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="8"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="26"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1425,15 +1445,15 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="8"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="26"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1446,17 +1466,17 @@
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="8"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="26"/>
       <c r="K28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -1470,15 +1490,15 @@
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="8"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="26"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1491,17 +1511,17 @@
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="2:21">
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="31" t="s">
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="8"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="6"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1514,15 +1534,15 @@
       <c r="U30" s="2"/>
     </row>
     <row r="31" spans="2:21">
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="8"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="6"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1535,15 +1555,15 @@
       <c r="U31" s="2"/>
     </row>
     <row r="32" spans="2:21">
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="8"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="6"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1556,15 +1576,15 @@
       <c r="U32" s="2"/>
     </row>
     <row r="33" spans="2:21">
-      <c r="B33" s="8"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="8"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="6"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1577,15 +1597,15 @@
       <c r="U33" s="2"/>
     </row>
     <row r="34" spans="2:21">
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="8"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="6"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -1598,15 +1618,15 @@
       <c r="U34" s="2"/>
     </row>
     <row r="35" spans="2:21">
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -1619,15 +1639,15 @@
       <c r="U35" s="2"/>
     </row>
     <row r="36" spans="2:21">
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -1639,16 +1659,16 @@
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
     </row>
-    <row r="37" spans="2:21">
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
+    <row r="37" spans="2:21" ht="11.25" customHeight="1">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -1661,17 +1681,17 @@
       <c r="U37" s="2"/>
     </row>
     <row r="38" spans="2:21">
-      <c r="B38" s="8"/>
-      <c r="C38" s="25" t="s">
-        <v>3</v>
+      <c r="B38" s="6"/>
+      <c r="C38" s="22" t="s">
+        <v>2</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -1684,15 +1704,15 @@
       <c r="U38" s="2"/>
     </row>
     <row r="39" spans="2:21">
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -1741,37 +1761,9 @@
       <c r="U42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D27:H27"/>
+  <mergeCells count="39">
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:H20"/>
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="B30:C30"/>
@@ -1779,6 +1771,36 @@
     <mergeCell ref="D31:H31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.70866141732283472" top="0.62992125984251968" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update TIR template Excel file to reflect recent changes in data structure and formatting
</commit_message>
<xml_diff>
--- a/backend/templates/TIR_template.xlsx
+++ b/backend/templates/TIR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Prodeklarant\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD6577B-A28E-47C4-87AB-D9E92FA4A6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAC721B-B914-4F2E-B62C-2F53F9CF6294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,11 +350,20 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="4"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,20 +377,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="4"/>
-    </xf>
-    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -834,8 +834,8 @@
   </sheetPr>
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -900,10 +900,10 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="6"/>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -925,8 +925,8 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="6"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -948,8 +948,8 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="6"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -1074,9 +1074,9 @@
       <c r="G10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
       <c r="K10" s="14"/>
       <c r="L10" s="20"/>
       <c r="M10" s="2"/>
@@ -1099,9 +1099,9 @@
       <c r="G11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="6"/>
       <c r="L11" s="21"/>
       <c r="M11" s="2"/>
@@ -1234,13 +1234,13 @@
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="24"/>
       <c r="J17" s="25"/>
       <c r="L17" s="2"/>
@@ -1255,13 +1255,13 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25"/>
       <c r="L18" s="2"/>
@@ -1276,13 +1276,13 @@
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="24"/>
       <c r="J19" s="25"/>
       <c r="L19" s="2"/>
@@ -1297,13 +1297,13 @@
       <c r="U19" s="2"/>
     </row>
     <row r="20" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
       <c r="I20" s="24"/>
       <c r="J20" s="25"/>
       <c r="L20" s="2"/>
@@ -1318,13 +1318,13 @@
       <c r="U20" s="2"/>
     </row>
     <row r="21" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
       <c r="I21" s="24"/>
       <c r="J21" s="26"/>
       <c r="K21" s="4"/>
@@ -1340,13 +1340,13 @@
       <c r="U21" s="5"/>
     </row>
     <row r="22" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
       <c r="I22" s="24"/>
       <c r="J22" s="26"/>
       <c r="L22" s="5"/>
@@ -1361,13 +1361,13 @@
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
       <c r="I23" s="24"/>
       <c r="J23" s="26"/>
       <c r="L23" s="5"/>
@@ -1382,13 +1382,13 @@
       <c r="U23" s="5"/>
     </row>
     <row r="24" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
       <c r="I24" s="24"/>
       <c r="J24" s="26"/>
       <c r="L24" s="5"/>
@@ -1403,13 +1403,13 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
       <c r="I25" s="24"/>
       <c r="J25" s="26"/>
       <c r="L25" s="5"/>
@@ -1424,13 +1424,13 @@
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
       <c r="I26" s="24"/>
       <c r="J26" s="26"/>
       <c r="L26" s="2"/>
@@ -1445,13 +1445,13 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="24"/>
       <c r="J27" s="26"/>
       <c r="L27" s="2"/>
@@ -1466,13 +1466,13 @@
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
       <c r="I28" s="24"/>
       <c r="J28" s="26"/>
       <c r="K28" s="1" t="s">
@@ -1490,13 +1490,13 @@
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
       <c r="I29" s="24"/>
       <c r="J29" s="26"/>
       <c r="L29" s="2"/>
@@ -1511,15 +1511,15 @@
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="2:21">
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="38" t="s">
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="7"/>
       <c r="J30" s="6"/>
       <c r="L30" s="2"/>
@@ -1534,13 +1534,13 @@
       <c r="U30" s="2"/>
     </row>
     <row r="31" spans="2:21">
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="7"/>
       <c r="J31" s="6"/>
       <c r="L31" s="2"/>
@@ -1555,13 +1555,13 @@
       <c r="U31" s="2"/>
     </row>
     <row r="32" spans="2:21">
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
       <c r="I32" s="7"/>
       <c r="J32" s="6"/>
       <c r="L32" s="2"/>
@@ -1579,9 +1579,9 @@
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
       <c r="H33" s="9"/>
       <c r="I33" s="10"/>
       <c r="J33" s="6"/>
@@ -1600,8 +1600,8 @@
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
       <c r="G34" s="11"/>
       <c r="H34" s="9"/>
       <c r="I34" s="12"/>
@@ -1762,6 +1762,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="E33:G33"/>
@@ -1778,29 +1801,6 @@
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E29:H29"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.70866141732283472" top="0.62992125984251968" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update TIR_template.xlsx and remove @floating-ui/dom from package-lock.json
- Updated the TIR_template.xlsx file to reflect recent changes.
- Removed the optional dependency for @floating-ui/dom from package-lock.json to streamline package management.
</commit_message>
<xml_diff>
--- a/backend/templates/TIR_template.xlsx
+++ b/backend/templates/TIR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Prodeklarant\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAC721B-B914-4F2E-B62C-2F53F9CF6294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCF1D88-7F87-4F10-A66A-B15CD647D428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,6 +350,24 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -364,24 +382,6 @@
     </xf>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -840,7 +840,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.140625" style="1" customWidth="1"/>
@@ -900,10 +900,10 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="6"/>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -925,8 +925,8 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="6"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -948,8 +948,8 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="6"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -1074,9 +1074,9 @@
       <c r="G10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
       <c r="K10" s="14"/>
       <c r="L10" s="20"/>
       <c r="M10" s="2"/>
@@ -1099,9 +1099,9 @@
       <c r="G11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="6"/>
       <c r="L11" s="21"/>
       <c r="M11" s="2"/>
@@ -1234,13 +1234,13 @@
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
       <c r="I17" s="24"/>
       <c r="J17" s="25"/>
       <c r="L17" s="2"/>
@@ -1255,13 +1255,13 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25"/>
       <c r="L18" s="2"/>
@@ -1276,13 +1276,13 @@
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
       <c r="I19" s="24"/>
       <c r="J19" s="25"/>
       <c r="L19" s="2"/>
@@ -1297,13 +1297,13 @@
       <c r="U19" s="2"/>
     </row>
     <row r="20" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
       <c r="I20" s="24"/>
       <c r="J20" s="25"/>
       <c r="L20" s="2"/>
@@ -1318,13 +1318,13 @@
       <c r="U20" s="2"/>
     </row>
     <row r="21" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="24"/>
       <c r="J21" s="26"/>
       <c r="K21" s="4"/>
@@ -1340,13 +1340,13 @@
       <c r="U21" s="5"/>
     </row>
     <row r="22" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
       <c r="I22" s="24"/>
       <c r="J22" s="26"/>
       <c r="L22" s="5"/>
@@ -1361,13 +1361,13 @@
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
       <c r="I23" s="24"/>
       <c r="J23" s="26"/>
       <c r="L23" s="5"/>
@@ -1382,13 +1382,13 @@
       <c r="U23" s="5"/>
     </row>
     <row r="24" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
       <c r="I24" s="24"/>
       <c r="J24" s="26"/>
       <c r="L24" s="5"/>
@@ -1403,13 +1403,13 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="2:21" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="24"/>
       <c r="J25" s="26"/>
       <c r="L25" s="5"/>
@@ -1424,13 +1424,13 @@
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="24"/>
       <c r="J26" s="26"/>
       <c r="L26" s="2"/>
@@ -1445,13 +1445,13 @@
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
       <c r="I27" s="24"/>
       <c r="J27" s="26"/>
       <c r="L27" s="2"/>
@@ -1466,13 +1466,13 @@
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
       <c r="I28" s="24"/>
       <c r="J28" s="26"/>
       <c r="K28" s="1" t="s">
@@ -1490,13 +1490,13 @@
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
       <c r="I29" s="24"/>
       <c r="J29" s="26"/>
       <c r="L29" s="2"/>
@@ -1511,15 +1511,15 @@
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="2:21">
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="32" t="s">
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
       <c r="I30" s="7"/>
       <c r="J30" s="6"/>
       <c r="L30" s="2"/>
@@ -1534,13 +1534,13 @@
       <c r="U30" s="2"/>
     </row>
     <row r="31" spans="2:21">
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="7"/>
       <c r="J31" s="6"/>
       <c r="L31" s="2"/>
@@ -1555,13 +1555,13 @@
       <c r="U31" s="2"/>
     </row>
     <row r="32" spans="2:21">
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="7"/>
       <c r="J32" s="6"/>
       <c r="L32" s="2"/>
@@ -1579,9 +1579,9 @@
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="9"/>
       <c r="I33" s="10"/>
       <c r="J33" s="6"/>
@@ -1600,8 +1600,8 @@
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="11"/>
       <c r="H34" s="9"/>
       <c r="I34" s="12"/>
@@ -1762,29 +1762,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="E33:G33"/>
@@ -1801,6 +1778,29 @@
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E29:H29"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.70866141732283472" top="0.62992125984251968" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>